<commit_message>
Added execution, summary, test cases, bug-updated reports
</commit_message>
<xml_diff>
--- a/QA_reports/TEST_EXECUSION_REPORT.xlsx
+++ b/QA_reports/TEST_EXECUSION_REPORT.xlsx
@@ -8,25 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechIN\5. Projektas\Ziemos_kodas_JV\Ziemos_kodas QA\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D07861-8F6F-4593-904D-479EBF3697FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE97CED-371A-4C22-A70C-0E4CE1FEA0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="2655" windowWidth="18975" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20025" yWindow="1500" windowWidth="14085" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1st_SPRINT" sheetId="1" r:id="rId1"/>
     <sheet name="2nd_SPRINT" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Field</t>
   </si>
@@ -55,9 +66,6 @@
     <t>Failed Test Cases</t>
   </si>
   <si>
-    <t>Test Environment</t>
-  </si>
-  <si>
     <t>Operating System</t>
   </si>
   <si>
@@ -67,9 +75,6 @@
     <t>Other Relevant Info</t>
   </si>
   <si>
-    <t>Test Summary</t>
-  </si>
-  <si>
     <t>Overall Status</t>
   </si>
   <si>
@@ -110,6 +115,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>1st SPRINT</t>
+  </si>
+  <si>
+    <t>2st SPRINT</t>
+  </si>
+  <si>
+    <t>22 (18 fixed- 4 refused)</t>
+  </si>
+  <si>
+    <t>29/12</t>
   </si>
 </sst>
 </file>
@@ -217,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +251,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -242,18 +274,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B21"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,113 +625,115 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5" t="s">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>27</v>
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="10"/>
+      <c r="A20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -721,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE0A15E-CDF1-4A32-8D1F-585DCB771CD4}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,111 +789,127 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
+      <c r="B15" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="10"/>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>